<commit_message>
CA documentation updated to use Install Params / Properties, and cleaned up a bit
</commit_message>
<xml_diff>
--- a/Documentation/AI Loud Install CA Usage.xlsx
+++ b/Documentation/AI Loud Install CA Usage.xlsx
@@ -1,24 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79A88BE9-4028-4187-BD9E-4831A329C16C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C8D85F-BB6D-44A5-BDFD-A08B31DCE333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23184" yWindow="3276" windowWidth="20916" windowHeight="17148" tabRatio="777" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="1872" yWindow="0" windowWidth="22392" windowHeight="14640" tabRatio="777" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="2" r:id="rId1"/>
     <sheet name="Define CAs to AI" sheetId="3" r:id="rId2"/>
     <sheet name="InitProps err dlg" sheetId="4" r:id="rId3"/>
-    <sheet name="InitProps sequence" sheetId="5" r:id="rId4"/>
-    <sheet name="call RemoveInstalled CA" sheetId="7" r:id="rId5"/>
-    <sheet name="RemoveInstalledErrDlg" sheetId="6" r:id="rId6"/>
+    <sheet name="RemoveInstalledErrDlg" sheetId="6" r:id="rId4"/>
+    <sheet name="Dialog sequence+conditions" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
   <si>
     <t>There is a companion AI installer in</t>
   </si>
@@ -55,9 +54,6 @@
     <t>If you choose to build it, at the very least the Build Output directories will need to be tailored to your enviroment.</t>
   </si>
   <si>
-    <t>3D-1902-Loud-FindIns-RemCAs.aip</t>
-  </si>
-  <si>
     <t>It pretends to be a RISA-3D installer - and installs some of the files 3D needs</t>
   </si>
   <si>
@@ -82,9 +78,6 @@
     <t>Start</t>
   </si>
   <si>
-    <t>Via the table editor, setup these properties --&gt;</t>
-  </si>
-  <si>
     <t>adding a Wix DTF custom action (at least one that's tied to a sequence) is detailed in AI's documentation:</t>
   </si>
   <si>
@@ -103,9 +96,6 @@
     <t>for both CAs, use the dialog below to integrate them into the installer via the "Call function from attached native DLL" choice:</t>
   </si>
   <si>
-    <t>Create the error handling dialog to handle problems detected in InitProperties</t>
-  </si>
-  <si>
     <t>Change "New Dialog" title to</t>
   </si>
   <si>
@@ -118,36 +108,18 @@
     <t xml:space="preserve">When this dialog is created, AI also creates a </t>
   </si>
   <si>
-    <t>The Cancel button's text should probably be</t>
-  </si>
-  <si>
     <t>&lt;--The confusing verbiage explained:</t>
   </si>
   <si>
     <t>CancelDialog that's fired when user presses Cancel</t>
   </si>
   <si>
-    <t>This is just a Y/N confirmation, are you sure</t>
-  </si>
-  <si>
-    <t>and set the Cancel button at left to fire it, short circuiting the call to this CancelDialog</t>
-  </si>
-  <si>
     <t>AI sees this, and removes CancelDialog from the dialog tree, in the leftmost part of the picture</t>
   </si>
   <si>
-    <t>changed to "Exit" or something final-sounding</t>
-  </si>
-  <si>
     <t>Getting the Cancel button to fire the correct event involves:</t>
   </si>
   <si>
-    <t>Goto the Table Editor and make final adjustments for InitProperties and its error dialog</t>
-  </si>
-  <si>
-    <t>Visit the Table Editor - and set the Dialog's Condition</t>
-  </si>
-  <si>
     <t>There is nothing sacrosanct about this installer, feel free to change it as needed.</t>
   </si>
   <si>
@@ -160,9 +132,6 @@
     <t>and selecting "Close the current dialog" from the choices</t>
   </si>
   <si>
-    <t>Hook up the RemoveInstalledProducts CA - recall that it is out of sequence and is triggered by event</t>
-  </si>
-  <si>
     <t>here we tell AI to call this CA when user presses "Install" on the "Ready to Install" dialog</t>
   </si>
   <si>
@@ -197,6 +166,81 @@
   </si>
   <si>
     <t>State set in this library, even though declared statically, can't be passed to the next CA that's called</t>
+  </si>
+  <si>
+    <t>In AI's Install Parameters screen, setup these properties --&gt;</t>
+  </si>
+  <si>
+    <t>RemoveInstalledProducts - make sure the CA references the RemoveInstalledProducts function, in the right hand pane (should be able to select it from the dropdown)</t>
+  </si>
+  <si>
+    <t>Add a New Dialog (in sequence)</t>
+  </si>
+  <si>
+    <t>make sure it's positioned as the first dialog under the "First Time Install" node</t>
+  </si>
+  <si>
+    <t>The Cancel button's text can be changed to "Exit" via a built-in property:</t>
+  </si>
+  <si>
+    <t>Change its name to RemoveInstalledProductsErrorDlg (name isn't important, just name it clearly)</t>
+  </si>
+  <si>
+    <t>Goto the Table Editor and make final adjustments for both error dialogs</t>
+  </si>
+  <si>
+    <t>set the dialog's:</t>
+  </si>
+  <si>
+    <t>Title control's Text to "An Error Occurred" or similar</t>
+  </si>
+  <si>
+    <t>Description control's Text to property [RISA_STATUS_TEXT]</t>
+  </si>
+  <si>
+    <t>Back and Next buttons to Visible = False</t>
+  </si>
+  <si>
+    <t>Cancel button to publish event "Close the current dialog"</t>
+  </si>
+  <si>
+    <t>Cancel button's text to Special Property / ButtonText_Exit</t>
+  </si>
+  <si>
+    <t>Hook up this dialog into the flow of events:</t>
+  </si>
+  <si>
+    <t>Hook up the RemoveInstalledProducts CA - recall that it is out of sequence and is triggered by an event - specified below</t>
+  </si>
+  <si>
+    <t>Finish customzing this dialog in the same fashion as InitPropsErrorDlg</t>
+  </si>
+  <si>
+    <t>This will cause the RemoveInstalledProducts CA to run when user hits "Install"</t>
+  </si>
+  <si>
+    <t>When the CA has returned, its error handling dialog, RemoveInstalledProductsErrorDlg is shown, if there was an error. This condition is specified next.</t>
+  </si>
+  <si>
+    <t>3D-1901-Loud-RunCAs-ShowErrorDialogs.aip</t>
+  </si>
+  <si>
+    <t>Create the error handling dialog to display RISA_STATUS_TEXT when problems are detected in the InitProperties CA</t>
+  </si>
+  <si>
+    <t>rename it to "InitPropertiesErrorDlg" (the name is not important, just something clear)</t>
+  </si>
+  <si>
+    <t>This is just a Y/N confirmation, "are you sure?" (we are, and don't want the confirmation dlg)</t>
+  </si>
+  <si>
+    <t>and set the Cancel button to fire it, short circuiting the call to the confirmation dialog</t>
+  </si>
+  <si>
+    <t>select the Cancel button (it was changed to display "Exit" on the button face)</t>
+  </si>
+  <si>
+    <t>choose a  "Special Property" - ButtonText_Exit</t>
   </si>
 </sst>
 </file>
@@ -301,23 +345,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>160020</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>196164</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>198121</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>220980</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>97074</xdr:rowOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>137159</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>144781</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{56FF5EC5-89E1-4C47-91E8-AD6E38D5D6B2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F4503F7E-04C6-4DDB-B33F-C5982E32EEA6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -339,8 +383,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4000500" y="3566160"/>
-          <a:ext cx="7261860" cy="3206034"/>
+          <a:off x="4516704" y="3535681"/>
+          <a:ext cx="7141895" cy="4198620"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -454,6 +498,56 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>53340</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
+      <xdr:row>70</xdr:row>
+      <xdr:rowOff>178349</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4E2E53D1-3D98-4170-B4D6-44C7B79E3E6F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1630680" y="11369040"/>
+          <a:ext cx="7772400" cy="1717589"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -463,13 +557,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>25</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>86082</xdr:colOff>
-      <xdr:row>36</xdr:row>
+      <xdr:row>57</xdr:row>
       <xdr:rowOff>47480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -513,13 +607,13 @@
     <xdr:from>
       <xdr:col>2</xdr:col>
       <xdr:colOff>129540</xdr:colOff>
-      <xdr:row>40</xdr:row>
+      <xdr:row>61</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
       <xdr:colOff>60960</xdr:colOff>
-      <xdr:row>60</xdr:row>
+      <xdr:row>81</xdr:row>
       <xdr:rowOff>131534</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -559,6 +653,106 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>282770</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>168672</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="7" name="Picture 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0AE6CB20-3046-441E-88A8-E4E5508B95F8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1249680" y="777240"/>
+          <a:ext cx="2782130" cy="3460512"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>182880</xdr:colOff>
+      <xdr:row>84</xdr:row>
+      <xdr:rowOff>144780</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>127</xdr:row>
+      <xdr:rowOff>118350</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="9" name="Picture 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1A11DAB0-2A84-423C-B9F7-2C24AAC14BF1}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1432560" y="16131540"/>
+          <a:ext cx="7772400" cy="7837410"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -566,23 +760,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>91440</xdr:rowOff>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>373380</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>143630</xdr:rowOff>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>121920</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>28640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2236BE35-81DB-45C9-B143-2092B317A06D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C0617D-1AB2-4DAD-8D30-F82E6801C47F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -604,8 +798,108 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="678180" y="1188720"/>
-          <a:ext cx="9502140" cy="4989950"/>
+          <a:off x="3497580" y="2255520"/>
+          <a:ext cx="8496300" cy="5652200"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>115080</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>100295</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947EC7CC-0DA5-47B7-AFCD-4A889962EC6E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="624840" y="563880"/>
+          <a:ext cx="2614440" cy="4138895"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>93</xdr:row>
+      <xdr:rowOff>158541</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Picture 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4885E64-DA9D-4007-BCF8-DF11352AB1D9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1249680" y="11628120"/>
+          <a:ext cx="7772400" cy="5644941"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -622,22 +916,22 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>53340</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>205739</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>167640</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>182880</xdr:colOff>
-      <xdr:row>43</xdr:row>
-      <xdr:rowOff>27978</xdr:rowOff>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>338226</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
+        <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{219305ED-FC11-4660-8581-F78D6C3691A2}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6E26391A-5C9B-47FD-BB47-05CF9B2B7030}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -659,113 +953,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="678180" y="990600"/>
-          <a:ext cx="9502140" cy="6901218"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>3</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>373380</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>165800</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Picture 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{90C0617D-1AB2-4DAD-8D30-F82E6801C47F}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="624840" y="548640"/>
-          <a:ext cx="8496300" cy="5652200"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>14</xdr:col>
-      <xdr:colOff>266700</xdr:colOff>
-      <xdr:row>72</xdr:row>
-      <xdr:rowOff>34785</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Picture 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D8C894C7-E425-4D13-A3DA-904960B508D6}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2">
-          <a:extLst>
-            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
-              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
-            </a:ext>
-          </a:extLst>
-        </a:blip>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="624840" y="6949440"/>
-          <a:ext cx="8389620" cy="6252705"/>
+          <a:off x="830579" y="1280160"/>
+          <a:ext cx="8255407" cy="5532120"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1077,7 +1266,7 @@
   <dimension ref="B2:R25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D35" sqref="D35"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1087,7 +1276,7 @@
   <sheetData>
     <row r="2" spans="2:18" ht="18" x14ac:dyDescent="0.35">
       <c r="B2" s="4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="2:18" x14ac:dyDescent="0.3">
@@ -1095,7 +1284,7 @@
         <v>0</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:18" x14ac:dyDescent="0.3">
@@ -1103,12 +1292,12 @@
         <v>1</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
       <c r="E5" s="1" t="s">
-        <v>5</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
@@ -1116,18 +1305,18 @@
         <v>2</v>
       </c>
       <c r="Q6" s="1" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="R6" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
     </row>
     <row r="8" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="R8" s="1" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="2:18" x14ac:dyDescent="0.3">
@@ -1135,15 +1324,15 @@
         <v>3</v>
       </c>
       <c r="R9" s="1" t="s">
-        <v>47</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C11" s="1" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="Q11" s="1" t="s">
-        <v>48</v>
+        <v>38</v>
       </c>
     </row>
     <row r="13" spans="2:18" x14ac:dyDescent="0.3">
@@ -1153,45 +1342,45 @@
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
       <c r="C15" s="1" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
       <c r="D16" s="1" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="E17" s="1" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="19" spans="2:5" ht="18" x14ac:dyDescent="0.35">
       <c r="B19" s="4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="20" spans="2:5" x14ac:dyDescent="0.3">
       <c r="C20" s="1" t="s">
-        <v>14</v>
+        <v>43</v>
       </c>
     </row>
     <row r="22" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="1" t="s">
         <v>7</v>
-      </c>
-      <c r="E22" s="1" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="24" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D24" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="25" spans="2:5" x14ac:dyDescent="0.3">
       <c r="D25" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -1202,10 +1391,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB26601-7D7D-4E98-B186-E684C91D2C5E}">
-  <dimension ref="B3:M31"/>
+  <dimension ref="B3:M61"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="7.6640625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1215,37 +1404,42 @@
   <sheetData>
     <row r="3" spans="2:13" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="2:13" x14ac:dyDescent="0.3">
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:13" x14ac:dyDescent="0.3">
       <c r="F6" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C8" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="2:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M12" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="22" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="M22" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="31" spans="3:13" ht="15.6" x14ac:dyDescent="0.3">
       <c r="C31" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C61" s="3" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
@@ -1256,10 +1450,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E414ED9C-1928-4B8B-8A39-0B525333A639}">
-  <dimension ref="B3:Q39"/>
+  <dimension ref="B3:Q101"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="U47" sqref="U47"/>
+      <selection activeCell="T91" sqref="T91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1270,84 +1464,104 @@
     <col min="17" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:16" ht="18" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:9" ht="18" x14ac:dyDescent="0.35">
       <c r="B3" s="4" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="H13" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I14" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I15" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="30" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P30" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="31" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P31" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P40" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="42" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P42" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="Q43" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="44" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="Q44" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="46" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P46" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="47" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P47" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="48" spans="16:17" x14ac:dyDescent="0.3">
+      <c r="P48" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="P54" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="55" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="Q55" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="56" spans="3:17" x14ac:dyDescent="0.3">
+      <c r="Q56" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="60" spans="3:17" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C60" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P10" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P12" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="2:16" x14ac:dyDescent="0.3">
-      <c r="P13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P19" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="21" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P21" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="22" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="Q22" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="23" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="Q23" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P25" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="26" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P26" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="27" spans="16:17" x14ac:dyDescent="0.3">
-      <c r="P27" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="33" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="P33" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="34" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="Q34" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="35" spans="3:17" x14ac:dyDescent="0.3">
-      <c r="Q35" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="39" spans="3:17" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C39" s="3" t="s">
-        <v>24</v>
+    <row r="84" spans="3:3" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C84" s="3" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="100" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q100" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="101" spans="17:17" x14ac:dyDescent="0.3">
+      <c r="Q101" s="1" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>
@@ -1357,11 +1571,116 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B777957-5B4B-497B-9684-D1B7BC6EFF1A}">
+  <dimension ref="B2:I99"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="R53" sqref="R53"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="9.109375" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="10" spans="2:7" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G10" s="3" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="G46" s="3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="H48" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I49" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="50" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I50" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="51" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="I51" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="52" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B52" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="54" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C54" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="55" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="D55" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="61" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B61" s="3" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="62" spans="2:9" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="C62" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="85" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="86" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="87" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="88" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="89" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="90" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="91" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="92" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="93" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="94" s="1" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B97" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="99" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="B99" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE321A4-441C-48C5-8806-0D2BE0AF6764}">
   <dimension ref="B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="M52" sqref="M52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1371,65 +1690,7 @@
   <sheetData>
     <row r="5" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B5" s="3" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E68FE72B-C424-4984-8C6B-18AE1F9FB3E3}">
-  <dimension ref="B3:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="Q42" sqref="Q42"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="3" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B3" s="3" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="4" spans="2:3" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="C4" s="3" t="s">
-        <v>41</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B777957-5B4B-497B-9684-D1B7BC6EFF1A}">
-  <dimension ref="B2:B37"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S22" sqref="S22"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="16384" width="9.109375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="B37" s="3" t="s">
-        <v>35</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
doc changes based on Tom's findings
</commit_message>
<xml_diff>
--- a/Documentation/AI Loud Install CA Usage.xlsx
+++ b/Documentation/AI Loud Install CA Usage.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Advanced Installer\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62C8D85F-BB6D-44A5-BDFD-A08B31DCE333}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47AC301F-29C4-4B5D-B346-33D33FE77DC2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1872" yWindow="0" windowWidth="22392" windowHeight="14640" tabRatio="777" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
+    <workbookView xWindow="-32688" yWindow="3000" windowWidth="25668" windowHeight="20640" tabRatio="777" activeTab="4" xr2:uid="{757481C7-A015-4B07-931A-B1A835412FCC}"/>
   </bookViews>
   <sheets>
     <sheet name="Start" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
   <si>
     <t>There is a companion AI installer in</t>
   </si>
@@ -241,6 +241,9 @@
   </si>
   <si>
     <t>choose a  "Special Property" - ButtonText_Exit</t>
+  </si>
+  <si>
+    <t>The above doesn't always work in real life. You can specify the condition in a panel adjacent to Custom Actions and Install Sequence:</t>
   </si>
 </sst>
 </file>
@@ -955,6 +958,56 @@
         <a:xfrm>
           <a:off x="830579" y="1280160"/>
           <a:ext cx="8255407" cy="5532120"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>274320</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>116601</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B9CD5D22-E271-48B3-B486-EE8EBB2D33E9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="624840" y="7513320"/>
+          <a:ext cx="7772400" cy="4688601"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1265,7 +1318,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA18370B-E1D7-4FC5-A726-A44356352CFF}">
   <dimension ref="B2:R25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
@@ -1393,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB26601-7D7D-4E98-B186-E684C91D2C5E}">
   <dimension ref="B3:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A19" workbookViewId="0">
       <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
@@ -1452,7 +1505,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E414ED9C-1928-4B8B-8A39-0B525333A639}">
   <dimension ref="B3:Q101"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A82" workbookViewId="0">
       <selection activeCell="T91" sqref="T91"/>
     </sheetView>
   </sheetViews>
@@ -1574,7 +1627,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B777957-5B4B-497B-9684-D1B7BC6EFF1A}">
   <dimension ref="B2:I99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A58" workbookViewId="0">
       <selection activeCell="R53" sqref="R53"/>
     </sheetView>
   </sheetViews>
@@ -1677,10 +1730,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ABE321A4-441C-48C5-8806-0D2BE0AF6764}">
-  <dimension ref="B5"/>
+  <dimension ref="B5:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M52" sqref="M52"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="P57" sqref="P57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1693,6 +1746,11 @@
         <v>49</v>
       </c>
     </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B40" s="1" t="s">
+        <v>68</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>